<commit_message>
Add auto-browser opening, improved error handling, and HTTPS certificate auto-detection
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ไม่เกี่ยวกับงาน\cursor\product search app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B50FBCA-7C5C-4A46-A3FD-85DEF55CCE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B24E03-17EB-4DD5-9165-CDD7A154036A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7044" yWindow="2664" windowWidth="15420" windowHeight="8688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -36,34 +36,217 @@
     <t>Photo</t>
   </si>
   <si>
-    <t xml:space="preserve">ใบตัด fast cut </t>
-  </si>
-  <si>
-    <t>ใบตัด super cut</t>
-  </si>
-  <si>
-    <t>ใบตัด fast cut sumo รูป 1, ใบตัด fast cut sumo 2</t>
-  </si>
-  <si>
-    <t>ใบตัด super cut sumo รูป 1, ใบตัด super cut sumo 2</t>
-  </si>
-  <si>
     <t>ใบตัด gp sumo รูป 1, ใบตัด gp sumo รูป 2</t>
   </si>
   <si>
-    <t>ใบตัด GP</t>
-  </si>
-  <si>
-    <t>ใบตัด turbo cut</t>
-  </si>
-  <si>
-    <t>ใบตัด gold cut</t>
-  </si>
-  <si>
     <t>ใบตัด gold cut sumo รูป 1, ใบตัด gold cut sumo รูป 2</t>
   </si>
   <si>
     <t>ใบตัด turbo cut sumo รูป 1, ใบตัด turbo cut sumo รูป 2</t>
+  </si>
+  <si>
+    <t>ใบตัด fast cut 4"x1m</t>
+  </si>
+  <si>
+    <t>ใบตัด super cut 4"x1m</t>
+  </si>
+  <si>
+    <t>ใบตัด GP 4"x1.2m</t>
+  </si>
+  <si>
+    <t>ใบตัด turbo cut  4"x1.2m</t>
+  </si>
+  <si>
+    <t>ใบตัด gold cut 4"x1m</t>
+  </si>
+  <si>
+    <t>ใบตัด power cut 4"x1m</t>
+  </si>
+  <si>
+    <t>ใบตัด fast cut sumo รูป 1, ใบตัด fast cut sumo รูป 2</t>
+  </si>
+  <si>
+    <t>ใบตัด power cut sumo รูป 1, ใบตัด power cut sumo รูป 2</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง A24R 4"x4m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC24R 4"x6m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว CERAGRAIN A24R 4"x4m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว CERACUT A24R 4"x6m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง A24R 4x4m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC24R 4x6m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว A24R 4x4m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว CERACUT24R 4x6m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัด super cut sumo รูป 1, ใบตัด super cut sumo รูป 2</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AC60 TOP SHARK AC60 4"x2m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC60P 4"x2m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว CERAGRAIN 60P 4"x2m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว CERAGRAIN 80J 4"x2m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง A24R 5"x6m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง 4x2m AC60 top shark sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC60P 4x2m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว 60P 4x2m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว 80J 4x2m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง A24R 5x6m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีแดง CERAGRAIN60 7x1.2m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีแดง CERAGRAIN60 7"x1.2m</t>
+  </si>
+  <si>
+    <t>ใบตัดสีเขียว CERAGRAIN 7x1.6m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีเขียว CERAGRAIN60 7"x1.6m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC24P 7"x6m</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีแดง AWC24P 7x6m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว AWC24P 7x6m sumo</t>
+  </si>
+  <si>
+    <t>ใบเจียรสีเขียว AWC24P 7"x6m</t>
+  </si>
+  <si>
+    <t>ใบตัดสีดำ AWC30PBF 7"x3m</t>
+  </si>
+  <si>
+    <t>ใบตัดสีดำ AWC30PBF 7x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดหรือเจียร WAC60TBF 7x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดใบเจียรสีแดง WAC60TPB 7"x3m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีดำ SUPER CUT 14" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีดำ SUPER CUT 16" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t>ใบตัดสีดำ ใย1ชั้น super cut 14x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีดำ ใย1ชั้น super cut 16x3m sumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีเขียว FAST CUT 14" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีเขียว FAST CUT 16" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t>ใบตัดสีเขียว ใย1ชั้น super cut 14x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีเขียว ใย1ชั้น super cut 16x3m sumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีแดง SUPER CUT 14" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีแดง TOP SHARK 14" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดสีแดง TOP SHARK 16" ใย 1 ชั้น </t>
+  </si>
+  <si>
+    <t>ใบตัดสีแดง ใย1ชั้น super cut 14x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดสีแดง ใย1ชั้น super cut 16x3m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชรสีฟ้า TURBO CUT 4"x1.2m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชรสีแดง FAST CUT 4"x1.2m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร turbo cut 4x1.2m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร fast cut 4x1.2m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร segment 4x1.8m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร segment 7x2.2m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร segment 9x2.6m sumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ใบตัดเพชร ใบตัดปูน 20407 SEGMENT 4"x1.8m </t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร ใบตัดปูน 20707 SEGMENT 7"x2.2m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร ใบตัดปูน 20907 SEGMENT 9"x2.6m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร ใบตัดปูน 30708 ARROW TURBO 7"x2.6m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร ใบตัดปูน 40712 TURBO 7"x1.8m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร ใบตัดปูน 40912 TURBO 7"x2.0m</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร arrow turbo 7x2.6m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร turbo 7x1.8m sumo</t>
+  </si>
+  <si>
+    <t>ใบตัดเพชร turbo 9x2m sumo</t>
   </si>
 </sst>
 </file>
@@ -99,10 +282,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,16 +570,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="49.77734375" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" customWidth="1"/>
+    <col min="3" max="3" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -412,10 +598,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -423,21 +609,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -447,8 +633,8 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -458,8 +644,349 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>